<commit_message>
replace way to handle auto migration and outdate
</commit_message>
<xml_diff>
--- a/api/tests/acceptance/scripts/target-profile-migrations/migration-test.xlsx
+++ b/api/tests/acceptance/scripts/target-profile-migrations/migration-test.xlsx
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3775" uniqueCount="1368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3776" uniqueCount="1368">
   <si>
     <t xml:space="preserve">Attention - merci de créer un nouveau fichier pour chaque responsable. En reprenant l'onglet PRO et l'onglet Profil cible spécial. L'onglet "Profil cible spécial" servira à chaque profil cible avec du capage multiforme et/ou des paliers.  
 </t>
@@ -408,10 +408,10 @@
     <t xml:space="preserve">Profil cible avec traitement automatique -&gt; MIGRATION AUTO</t>
   </si>
   <si>
+    <t xml:space="preserve">Oui</t>
+  </si>
+  <si>
     <t xml:space="preserve">Profil cible sans capage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oui</t>
   </si>
   <si>
     <t xml:space="preserve">Profil cible avec capage uniforme</t>
@@ -5074,7 +5074,7 @@
       <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="76.13"/>
@@ -6294,7 +6294,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="71.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="55.88"/>
@@ -6667,10 +6667,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topRight" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.52"/>
@@ -6830,7 +6830,9 @@
       <c r="E4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="40"/>
+      <c r="F4" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
       <c r="I4" s="41"/>
@@ -6856,7 +6858,7 @@
         <v>42</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
@@ -6874,7 +6876,7 @@
         <v>2003</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>42</v>
@@ -6883,10 +6885,10 @@
         <v>42</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="41"/>
       <c r="I6" s="41"/>
@@ -6912,7 +6914,7 @@
         <v>42</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="41" t="s">
         <v>43</v>
@@ -6943,14 +6945,14 @@
         <v>42</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>43</v>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J8" s="42" t="s">
         <v>42</v>
@@ -6974,14 +6976,14 @@
         <v>42</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="41" t="s">
         <v>43</v>
       </c>
       <c r="H9" s="41"/>
       <c r="I9" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J9" s="42" t="s">
         <v>42</v>
@@ -7003,14 +7005,14 @@
         <v>42</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="41" t="s">
         <v>43</v>
       </c>
       <c r="H10" s="41"/>
       <c r="I10" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J10" s="42"/>
       <c r="K10" s="43"/>
@@ -7027,14 +7029,14 @@
         <v>42</v>
       </c>
       <c r="F11" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G11" s="41" t="s">
         <v>43</v>
       </c>
       <c r="H11" s="41"/>
       <c r="I11" s="41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J11" s="42"/>
       <c r="K11" s="43"/>
@@ -7850,7 +7852,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.13"/>
@@ -8941,7 +8943,7 @@
       <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="77.63"/>
@@ -30095,7 +30097,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">

</xml_diff>